<commit_message>
Updated all Scripts Waits&Sleeps
</commit_message>
<xml_diff>
--- a/data/UserSignInFunctionality.xlsx
+++ b/data/UserSignInFunctionality.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2(WORK)\Onelern\Automation\Frugal_Onelern_Structure\Frugal_Onelern_Structure\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C5968F-58E6-4E78-AE1C-117B1DCC55EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05488A2B-6FEC-4C7F-B83F-3B80D971F7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="827" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="827" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Student Credentials" sheetId="2" r:id="rId1"/>
@@ -368,7 +368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCADF823-0373-42FD-B1AC-D252257E245E}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -435,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D5921FD-4D90-40A0-A53C-89C97112D70F}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,7 +458,7 @@
         <v>9000000101</v>
       </c>
       <c r="B2" s="1">
-        <v>123465</v>
+        <v>123456</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -466,7 +466,7 @@
         <v>9000000105</v>
       </c>
       <c r="B3" s="1">
-        <v>123465</v>
+        <v>123456</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -474,7 +474,7 @@
         <v>9000000109</v>
       </c>
       <c r="B4" s="1">
-        <v>123465</v>
+        <v>123456</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -482,7 +482,7 @@
         <v>9000000113</v>
       </c>
       <c r="B5" s="1">
-        <v>123465</v>
+        <v>123456</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -490,7 +490,7 @@
         <v>9000000117</v>
       </c>
       <c r="B6" s="1">
-        <v>123465</v>
+        <v>123456</v>
       </c>
     </row>
   </sheetData>
@@ -707,7 +707,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B6"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>